<commit_message>
Changed item card charging into item points. Change leveling up into skill points. Add buy cost for upgrade cards.
</commit_message>
<xml_diff>
--- a/sheet/AttributeCardData.xlsx
+++ b/sheet/AttributeCardData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\datasheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E5D483-25D0-40AA-B174-EF72FF5300C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7839720C-96CA-4B36-9120-FABA58CC85B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6225" yWindow="3795" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>cardName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>vigor.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>agility.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -80,6 +76,34 @@
   </si>
   <si>
     <t>intelligence.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strength</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitality.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agility</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Awareness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intelligence</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,81 +429,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Card changes: Changed card count of most loot card and event card. Changed card count of attribute cards from 5 to 3. Changed the effect of Midas Touch and Genocide. Changed the effect of Sludge. Changed the buy cost of attribute card from 3 to 2.
</commit_message>
<xml_diff>
--- a/sheet/AttributeCardData.xlsx
+++ b/sheet/AttributeCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7839720C-96CA-4B36-9120-FABA58CC85B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AAFCF6-2860-4168-AFF4-34DD5C4F7174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -459,10 +459,10 @@
         <v>2</v>
       </c>
       <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
         <v>3</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -476,10 +476,10 @@
         <v>6</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>3</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -493,10 +493,10 @@
         <v>3</v>
       </c>
       <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>3</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -510,10 +510,10 @@
         <v>4</v>
       </c>
       <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>3</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -527,10 +527,10 @@
         <v>5</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>3</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Moved buy cost of upgrade card to the center.
</commit_message>
<xml_diff>
--- a/sheet/AttributeCardData.xlsx
+++ b/sheet/AttributeCardData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AAFCF6-2860-4168-AFF4-34DD5C4F7174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370EF64C-EFA6-48BC-9AA2-4CA470FD16D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,10 +79,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Strength</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,6 +100,10 @@
   </si>
   <si>
     <t>Intelligence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -432,7 +432,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -442,7 +442,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -465,7 +465,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -482,10 +482,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -533,7 +533,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>

</xml_diff>